<commit_message>
with SEIT A database
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">roll_no</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mohak Borole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elon Musk</t>
   </si>
 </sst>
 </file>
@@ -216,15 +213,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>8888848291</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>

</xml_diff>